<commit_message>
(fix): correction in time intervals
</commit_message>
<xml_diff>
--- a/VRPTW_LuisaMariaAlvarez_constructive.xlsx
+++ b/VRPTW_LuisaMariaAlvarez_constructive.xlsx
@@ -587,7 +587,7 @@
         <v>2711.296</v>
       </c>
       <c r="C1" t="n">
-        <v>12.005</v>
+        <v>62.391</v>
       </c>
     </row>
     <row r="2">
@@ -610,10 +610,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>4.243</v>
+        <v>86</v>
       </c>
       <c r="H2" t="n">
-        <v>106</v>
+        <v>192</v>
       </c>
       <c r="I2" t="n">
         <v>209.616</v>
@@ -654,16 +654,16 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>9.220000000000001</v>
+        <v>41</v>
       </c>
       <c r="L3" t="n">
         <v>56</v>
       </c>
       <c r="M3" t="n">
-        <v>72.325</v>
+        <v>91</v>
       </c>
       <c r="N3" t="n">
-        <v>112.18</v>
+        <v>155</v>
       </c>
       <c r="O3" t="n">
         <v>182.464</v>
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>10</v>
+        <v>144</v>
       </c>
       <c r="I4" t="n">
         <v>164</v>
@@ -745,7 +745,7 @@
         <v>11.18</v>
       </c>
       <c r="J5" t="n">
-        <v>27.888</v>
+        <v>133</v>
       </c>
       <c r="K5" t="n">
         <v>152.22</v>
@@ -783,10 +783,10 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>12.042</v>
+        <v>86</v>
       </c>
       <c r="I6" t="n">
-        <v>102.325</v>
+        <v>139</v>
       </c>
       <c r="J6" t="n">
         <v>155</v>
@@ -830,10 +830,10 @@
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>14.765</v>
+        <v>42</v>
       </c>
       <c r="L7" t="n">
-        <v>60.062</v>
+        <v>77</v>
       </c>
       <c r="M7" t="n">
         <v>97.77</v>
@@ -842,7 +842,7 @@
         <v>116.825</v>
       </c>
       <c r="O7" t="n">
-        <v>130.948</v>
+        <v>141</v>
       </c>
       <c r="P7" t="n">
         <v>162.18</v>
@@ -886,7 +886,7 @@
         <v>14.765</v>
       </c>
       <c r="K8" t="n">
-        <v>31.168</v>
+        <v>95</v>
       </c>
       <c r="L8" t="n">
         <v>124</v>
@@ -930,16 +930,16 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>15.811</v>
+        <v>66</v>
       </c>
       <c r="J9" t="n">
         <v>92.401</v>
       </c>
       <c r="K9" t="n">
-        <v>112.3</v>
+        <v>124</v>
       </c>
       <c r="L9" t="n">
-        <v>137.606</v>
+        <v>139</v>
       </c>
       <c r="M9" t="n">
         <v>193.204</v>
@@ -980,7 +980,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>17.889</v>
+        <v>67</v>
       </c>
       <c r="L10" t="n">
         <v>93.125</v>
@@ -1036,13 +1036,13 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>19.235</v>
+        <v>35</v>
       </c>
       <c r="L11" t="n">
         <v>53.062</v>
       </c>
       <c r="M11" t="n">
-        <v>77.20399999999999</v>
+        <v>83</v>
       </c>
       <c r="N11" t="n">
         <v>101.544</v>
@@ -1089,7 +1089,7 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>20.616</v>
+        <v>34</v>
       </c>
       <c r="K12" t="n">
         <v>53.22</v>
@@ -1139,13 +1139,13 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="K13" t="n">
-        <v>76.318</v>
+        <v>90</v>
       </c>
       <c r="L13" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="M13" t="n">
         <v>147.029</v>
@@ -1186,16 +1186,16 @@
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>27.459</v>
+        <v>30</v>
       </c>
       <c r="J14" t="n">
-        <v>55.033</v>
+        <v>75</v>
       </c>
       <c r="K14" t="n">
         <v>90.38500000000001</v>
       </c>
       <c r="L14" t="n">
-        <v>105.385</v>
+        <v>128</v>
       </c>
       <c r="M14" t="n">
         <v>176.079</v>
@@ -1230,10 +1230,10 @@
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>30.806</v>
+        <v>50</v>
       </c>
       <c r="J15" t="n">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="K15" t="n">
         <v>108</v>
@@ -1268,7 +1268,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>31.623</v>
+        <v>119</v>
       </c>
       <c r="H16" t="n">
         <v>168.217</v>
@@ -1309,7 +1309,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>32.388</v>
+        <v>64</v>
       </c>
       <c r="K17" t="n">
         <v>79</v>
@@ -1356,7 +1356,7 @@
         <v>33.541</v>
       </c>
       <c r="I18" t="n">
-        <v>45.541</v>
+        <v>64</v>
       </c>
       <c r="J18" t="n">
         <v>114.05</v>
@@ -1391,13 +1391,13 @@
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="I19" t="n">
         <v>105.606</v>
       </c>
       <c r="J19" t="n">
-        <v>141.568</v>
+        <v>144</v>
       </c>
       <c r="K19" t="n">
         <v>206.479</v>
@@ -1479,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>36.056</v>
+        <v>37</v>
       </c>
       <c r="I21" t="n">
         <v>54.071</v>
@@ -1552,7 +1552,7 @@
         <v>39.051</v>
       </c>
       <c r="I23" t="n">
-        <v>58.485</v>
+        <v>75</v>
       </c>
       <c r="J23" t="n">
         <v>102.464</v>
@@ -1584,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>40.05</v>
+        <v>72</v>
       </c>
       <c r="H24" t="n">
         <v>87.38500000000001</v>
@@ -1619,7 +1619,7 @@
         <v>42.426</v>
       </c>
       <c r="H25" t="n">
-        <v>68.23699999999999</v>
+        <v>74</v>
       </c>
       <c r="I25" t="n">
         <v>141.009</v>
@@ -1645,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>45.044</v>
+        <v>65</v>
       </c>
       <c r="G26" t="n">
         <v>120.044</v>
@@ -1677,7 +1677,7 @@
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>50.289</v>
+        <v>61</v>
       </c>
       <c r="I27" t="n">
         <v>73</v>
@@ -1718,7 +1718,7 @@
         <v>51.478</v>
       </c>
       <c r="I28" t="n">
-        <v>67.309</v>
+        <v>74</v>
       </c>
       <c r="J28" t="n">
         <v>88</v>
@@ -1757,7 +1757,7 @@
         <v>2468.243</v>
       </c>
       <c r="C1" t="n">
-        <v>12.128</v>
+        <v>92.553</v>
       </c>
     </row>
     <row r="2">
@@ -1792,10 +1792,10 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>4.243</v>
+        <v>359</v>
       </c>
       <c r="L2" t="n">
-        <v>379</v>
+        <v>822</v>
       </c>
       <c r="M2" t="n">
         <v>837.385</v>
@@ -1860,16 +1860,16 @@
         <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>9.220000000000001</v>
+        <v>157</v>
       </c>
       <c r="P3" t="n">
         <v>172</v>
       </c>
       <c r="Q3" t="n">
-        <v>188.325</v>
+        <v>375</v>
       </c>
       <c r="R3" t="n">
-        <v>396.18</v>
+        <v>694</v>
       </c>
       <c r="S3" t="n">
         <v>719</v>
@@ -1931,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>10</v>
+        <v>612</v>
       </c>
       <c r="M4" t="n">
         <v>637</v>
@@ -1999,25 +1999,25 @@
         <v>11.18</v>
       </c>
       <c r="N5" t="n">
-        <v>29.724</v>
+        <v>152</v>
       </c>
       <c r="O5" t="n">
-        <v>170.062</v>
+        <v>308</v>
       </c>
       <c r="P5" t="n">
-        <v>328.77</v>
+        <v>397</v>
       </c>
       <c r="Q5" t="n">
         <v>416.055</v>
       </c>
       <c r="R5" t="n">
-        <v>430.178</v>
+        <v>645</v>
       </c>
       <c r="S5" t="n">
         <v>676.213</v>
       </c>
       <c r="T5" t="n">
-        <v>697.393</v>
+        <v>703</v>
       </c>
       <c r="U5" t="n">
         <v>753.311</v>
@@ -2058,7 +2058,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>12.042</v>
+        <v>355</v>
       </c>
       <c r="L6" t="n">
         <v>373.062</v>
@@ -2067,10 +2067,10 @@
         <v>399.463</v>
       </c>
       <c r="N6" t="n">
-        <v>419.362</v>
+        <v>557</v>
       </c>
       <c r="O6" t="n">
-        <v>570.606</v>
+        <v>657</v>
       </c>
       <c r="P6" t="n">
         <v>679</v>
@@ -2117,10 +2117,10 @@
         <v>14.765</v>
       </c>
       <c r="L7" t="n">
-        <v>31.168</v>
+        <v>392</v>
       </c>
       <c r="M7" t="n">
-        <v>416.765</v>
+        <v>557</v>
       </c>
       <c r="N7" t="n">
         <v>588.5410000000001</v>
@@ -2176,10 +2176,10 @@
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>17.889</v>
+        <v>260</v>
       </c>
       <c r="N8" t="n">
-        <v>286.125</v>
+        <v>365</v>
       </c>
       <c r="O8" t="n">
         <v>382.211</v>
@@ -2191,7 +2191,7 @@
         <v>425.047</v>
       </c>
       <c r="R8" t="n">
-        <v>440.047</v>
+        <v>489</v>
       </c>
       <c r="S8" t="n">
         <v>505.403</v>
@@ -2250,13 +2250,13 @@
         <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>19.235</v>
+        <v>105</v>
       </c>
       <c r="P9" t="n">
-        <v>123.062</v>
+        <v>191</v>
       </c>
       <c r="Q9" t="n">
-        <v>213.042</v>
+        <v>395</v>
       </c>
       <c r="R9" t="n">
         <v>413.485</v>
@@ -2327,13 +2327,13 @@
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>20.616</v>
+        <v>100</v>
       </c>
       <c r="O10" t="n">
-        <v>119.22</v>
+        <v>167</v>
       </c>
       <c r="P10" t="n">
-        <v>184.071</v>
+        <v>268</v>
       </c>
       <c r="Q10" t="n">
         <v>291.038</v>
@@ -2383,10 +2383,10 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>25</v>
+        <v>175</v>
       </c>
       <c r="I11" t="n">
-        <v>199.318</v>
+        <v>359</v>
       </c>
       <c r="J11" t="n">
         <v>406.216</v>
@@ -2433,7 +2433,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>27.459</v>
+        <v>60</v>
       </c>
       <c r="M12" t="n">
         <v>85.297</v>
@@ -2442,7 +2442,7 @@
         <v>100.297</v>
       </c>
       <c r="O12" t="n">
-        <v>112.297</v>
+        <v>217</v>
       </c>
       <c r="P12" t="n">
         <v>260.734</v>
@@ -2495,7 +2495,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>33.526</v>
+        <v>195</v>
       </c>
       <c r="M13" t="n">
         <v>211</v>
@@ -2557,13 +2557,13 @@
         <v>35.355</v>
       </c>
       <c r="L14" t="n">
-        <v>48.355</v>
+        <v>105</v>
       </c>
       <c r="M14" t="n">
         <v>141.249</v>
       </c>
       <c r="N14" t="n">
-        <v>229.887</v>
+        <v>246</v>
       </c>
       <c r="O14" t="n">
         <v>260</v>
@@ -2610,7 +2610,7 @@
         <v>37.736</v>
       </c>
       <c r="K15" t="n">
-        <v>50.736</v>
+        <v>73</v>
       </c>
       <c r="L15" t="n">
         <v>128</v>
@@ -2651,7 +2651,7 @@
         <v>39.051</v>
       </c>
       <c r="H16" t="n">
-        <v>69.667</v>
+        <v>80</v>
       </c>
       <c r="I16" t="n">
         <v>141.478</v>
@@ -2687,7 +2687,7 @@
         <v>612.197</v>
       </c>
       <c r="C1" t="n">
-        <v>0.825</v>
+        <v>15.64</v>
       </c>
     </row>
     <row r="2">
@@ -2725,7 +2725,7 @@
         <v>196.434</v>
       </c>
       <c r="L2" t="n">
-        <v>294.244</v>
+        <v>2983</v>
       </c>
       <c r="M2" t="n">
         <v>3084.662</v>
@@ -2751,7 +2751,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>11.662</v>
+        <v>2887</v>
       </c>
       <c r="G3" t="n">
         <v>2988.662</v>
@@ -2795,25 +2795,25 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>15.133</v>
+        <v>25</v>
       </c>
       <c r="M4" t="n">
-        <v>120.831</v>
+        <v>213</v>
       </c>
       <c r="N4" t="n">
         <v>311.602</v>
       </c>
       <c r="O4" t="n">
-        <v>409.412</v>
+        <v>1073</v>
       </c>
       <c r="P4" t="n">
         <v>1167.123</v>
       </c>
       <c r="Q4" t="n">
-        <v>1260.729</v>
+        <v>1261</v>
       </c>
       <c r="R4" t="n">
-        <v>1376</v>
+        <v>2791</v>
       </c>
       <c r="S4" t="n">
         <v>2897.763</v>
@@ -2839,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>19.647</v>
+        <v>2698</v>
       </c>
       <c r="G5" t="n">
         <v>2807.647</v>
@@ -2865,7 +2865,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>23.324</v>
+        <v>2601</v>
       </c>
       <c r="G6" t="n">
         <v>2714.324</v>
@@ -2891,7 +2891,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>24.083</v>
+        <v>2504</v>
       </c>
       <c r="G7" t="n">
         <v>2618.083</v>
@@ -2929,16 +2929,16 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>25.298</v>
+        <v>497</v>
       </c>
       <c r="K8" t="n">
-        <v>611.083</v>
+        <v>1643</v>
       </c>
       <c r="L8" t="n">
         <v>1742.055</v>
       </c>
       <c r="M8" t="n">
-        <v>1835.055</v>
+        <v>2311</v>
       </c>
       <c r="N8" t="n">
         <v>2405</v>
@@ -2967,7 +2967,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>36.056</v>
+        <v>2216</v>
       </c>
       <c r="G9" t="n">
         <v>2342.056</v>
@@ -2993,7 +2993,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>38.079</v>
+        <v>2119</v>
       </c>
       <c r="G10" t="n">
         <v>2247.079</v>
@@ -3025,7 +3025,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>39.051</v>
+        <v>1837</v>
       </c>
       <c r="I11" t="n">
         <v>1934.071</v>
@@ -3067,7 +3067,7 @@
         <v>947.158</v>
       </c>
       <c r="C1" t="n">
-        <v>1.614</v>
+        <v>15.54</v>
       </c>
     </row>
     <row r="2">
@@ -3090,10 +3090,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>11.18</v>
+        <v>99</v>
       </c>
       <c r="H2" t="n">
-        <v>116.071</v>
+        <v>159</v>
       </c>
       <c r="I2" t="n">
         <v>180.18</v>
@@ -3128,13 +3128,13 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="J3" t="n">
-        <v>84.18000000000001</v>
+        <v>116</v>
       </c>
       <c r="K3" t="n">
-        <v>140.142</v>
+        <v>153</v>
       </c>
       <c r="L3" t="n">
         <v>178</v>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>15.232</v>
+        <v>161</v>
       </c>
       <c r="G4" t="n">
         <v>186.232</v>
@@ -3192,10 +3192,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>15.811</v>
+        <v>87</v>
       </c>
       <c r="H5" t="n">
-        <v>115.028</v>
+        <v>157</v>
       </c>
       <c r="I5" t="n">
         <v>197.414</v>
@@ -3227,13 +3227,13 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="I6" t="n">
         <v>70.44</v>
       </c>
       <c r="J6" t="n">
-        <v>90.44</v>
+        <v>149</v>
       </c>
       <c r="K6" t="n">
         <v>184</v>
@@ -3265,10 +3265,10 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>20.616</v>
+        <v>34</v>
       </c>
       <c r="I7" t="n">
-        <v>55.18</v>
+        <v>75</v>
       </c>
       <c r="J7" t="n">
         <v>129.721</v>
@@ -3300,7 +3300,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>21.213</v>
+        <v>81</v>
       </c>
       <c r="H8" t="n">
         <v>103.207</v>
@@ -3329,7 +3329,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>26.926</v>
+        <v>97</v>
       </c>
       <c r="G9" t="n">
         <v>133.926</v>
@@ -3358,7 +3358,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>30.414</v>
+        <v>61</v>
       </c>
       <c r="H10" t="n">
         <v>132.847</v>
@@ -3387,7 +3387,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>32.016</v>
+        <v>97</v>
       </c>
       <c r="G11" t="n">
         <v>139.016</v>
@@ -3439,7 +3439,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>32.016</v>
+        <v>76</v>
       </c>
       <c r="G13" t="n">
         <v>118.016</v>
@@ -3465,7 +3465,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>33.541</v>
+        <v>67</v>
       </c>
       <c r="G14" t="n">
         <v>110.541</v>
@@ -3491,7 +3491,7 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>36.056</v>
+        <v>68</v>
       </c>
       <c r="G15" t="n">
         <v>114.056</v>
@@ -3527,7 +3527,7 @@
         <v>737.55</v>
       </c>
       <c r="C1" t="n">
-        <v>1.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -3559,16 +3559,16 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>11.18</v>
+        <v>415</v>
       </c>
       <c r="K2" t="n">
-        <v>432.071</v>
+        <v>690</v>
       </c>
       <c r="L2" t="n">
         <v>725.495</v>
       </c>
       <c r="M2" t="n">
-        <v>745.495</v>
+        <v>817</v>
       </c>
       <c r="N2" t="n">
         <v>842</v>
@@ -3606,13 +3606,13 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>15</v>
+        <v>228</v>
       </c>
       <c r="J3" t="n">
-        <v>249.18</v>
+        <v>527</v>
       </c>
       <c r="K3" t="n">
-        <v>551.5599999999999</v>
+        <v>707</v>
       </c>
       <c r="L3" t="n">
         <v>757.706</v>
@@ -3653,7 +3653,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>15.811</v>
+        <v>377</v>
       </c>
       <c r="K4" t="n">
         <v>397</v>
@@ -3662,7 +3662,7 @@
         <v>419.207</v>
       </c>
       <c r="M4" t="n">
-        <v>455.456</v>
+        <v>577</v>
       </c>
       <c r="N4" t="n">
         <v>602.811</v>
@@ -3700,13 +3700,13 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>18</v>
+        <v>143</v>
       </c>
       <c r="J5" t="n">
-        <v>163.44</v>
+        <v>214</v>
       </c>
       <c r="K5" t="n">
-        <v>234</v>
+        <v>409</v>
       </c>
       <c r="L5" t="n">
         <v>469.99</v>
@@ -3741,10 +3741,10 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>20.616</v>
+        <v>34</v>
       </c>
       <c r="I6" t="n">
-        <v>55.18</v>
+        <v>272</v>
       </c>
       <c r="J6" t="n">
         <v>322.311</v>
@@ -3779,7 +3779,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>30.414</v>
+        <v>175</v>
       </c>
       <c r="I7" t="n">
         <v>200.811</v>
@@ -3811,7 +3811,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>33.541</v>
+        <v>206</v>
       </c>
       <c r="G8" t="n">
         <v>249.541</v>
@@ -3847,7 +3847,7 @@
         <v>859.181</v>
       </c>
       <c r="C1" t="n">
-        <v>0.997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -3879,16 +3879,16 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>30.806</v>
+        <v>50</v>
       </c>
       <c r="K2" t="n">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="L2" t="n">
         <v>108</v>
       </c>
       <c r="M2" t="n">
-        <v>125.071</v>
+        <v>141</v>
       </c>
       <c r="N2" t="n">
         <v>158.071</v>
@@ -3923,10 +3923,10 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>31.623</v>
+        <v>119</v>
       </c>
       <c r="I3" t="n">
-        <v>136.071</v>
+        <v>142</v>
       </c>
       <c r="J3" t="n">
         <v>163.18</v>
@@ -3967,7 +3967,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>32.388</v>
+        <v>64</v>
       </c>
       <c r="K4" t="n">
         <v>79</v>
@@ -3976,7 +3976,7 @@
         <v>94.38500000000001</v>
       </c>
       <c r="M4" t="n">
-        <v>138.794</v>
+        <v>148</v>
       </c>
       <c r="N4" t="n">
         <v>168.44</v>
@@ -4008,10 +4008,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="H5" t="n">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="I5" t="n">
         <v>167.057</v>
@@ -4049,10 +4049,10 @@
         <v>35.355</v>
       </c>
       <c r="J6" t="n">
-        <v>51.186</v>
+        <v>58</v>
       </c>
       <c r="K6" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L6" t="n">
         <v>132.09</v>
@@ -4081,7 +4081,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>39.051</v>
+        <v>91</v>
       </c>
       <c r="G7" t="n">
         <v>140.051</v>
@@ -4110,7 +4110,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>40.05</v>
+        <v>72</v>
       </c>
       <c r="H8" t="n">
         <v>87.38500000000001</v>
@@ -4139,7 +4139,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>40.311</v>
+        <v>41</v>
       </c>
       <c r="G9" t="n">
         <v>91.31100000000001</v>
@@ -4168,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="H10" t="n">
         <v>79</v>
@@ -4207,7 +4207,7 @@
         <v>839.2859999999999</v>
       </c>
       <c r="C1" t="n">
-        <v>0.393</v>
+        <v>15.622</v>
       </c>
     </row>
     <row r="2">
@@ -4254,10 +4254,10 @@
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>30.806</v>
+        <v>152</v>
       </c>
       <c r="P2" t="n">
-        <v>166</v>
+        <v>388</v>
       </c>
       <c r="Q2" t="n">
         <v>401</v>
@@ -4266,10 +4266,10 @@
         <v>416</v>
       </c>
       <c r="S2" t="n">
-        <v>431</v>
+        <v>644</v>
       </c>
       <c r="T2" t="n">
-        <v>661.071</v>
+        <v>673</v>
       </c>
       <c r="U2" t="n">
         <v>730.17</v>
@@ -4310,7 +4310,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>31.623</v>
+        <v>519</v>
       </c>
       <c r="H3" t="n">
         <v>569.6079999999999</v>
@@ -4354,13 +4354,13 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>32.388</v>
+        <v>223</v>
       </c>
       <c r="L4" t="n">
         <v>238</v>
       </c>
       <c r="M4" t="n">
-        <v>253.385</v>
+        <v>371</v>
       </c>
       <c r="N4" t="n">
         <v>417.056</v>
@@ -4410,10 +4410,10 @@
         <v>35.355</v>
       </c>
       <c r="K5" t="n">
-        <v>51.186</v>
+        <v>174</v>
       </c>
       <c r="L5" t="n">
-        <v>186</v>
+        <v>255</v>
       </c>
       <c r="M5" t="n">
         <v>316.614</v>
@@ -4448,10 +4448,10 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>40.311</v>
+        <v>73</v>
       </c>
       <c r="H6" t="n">
-        <v>165</v>
+        <v>201</v>
       </c>
       <c r="I6" t="n">
         <v>256.044</v>
@@ -4487,7 +4487,7 @@
         <v>811.437</v>
       </c>
       <c r="C1" t="n">
-        <v>4.878</v>
+        <v>46.805</v>
       </c>
     </row>
     <row r="2">
@@ -4516,10 +4516,10 @@
         <v>10</v>
       </c>
       <c r="I2" t="n">
-        <v>102</v>
+        <v>914</v>
       </c>
       <c r="J2" t="n">
-        <v>1021</v>
+        <v>1054</v>
       </c>
       <c r="K2" t="n">
         <v>1162.028</v>
@@ -4548,10 +4548,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>12.166</v>
+        <v>812</v>
       </c>
       <c r="H3" t="n">
-        <v>919</v>
+        <v>1001</v>
       </c>
       <c r="I3" t="n">
         <v>1110.209</v>
@@ -4580,10 +4580,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>13</v>
+        <v>732</v>
       </c>
       <c r="H4" t="n">
-        <v>843.401</v>
+        <v>912</v>
       </c>
       <c r="I4" t="n">
         <v>1020.682</v>
@@ -4627,22 +4627,22 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="M5" t="n">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="N5" t="n">
         <v>261</v>
       </c>
       <c r="O5" t="n">
-        <v>354</v>
+        <v>546</v>
       </c>
       <c r="P5" t="n">
         <v>638</v>
       </c>
       <c r="Q5" t="n">
-        <v>747.723</v>
+        <v>751</v>
       </c>
       <c r="R5" t="n">
         <v>863.204</v>
@@ -4686,10 +4686,10 @@
         <v>106.133</v>
       </c>
       <c r="K6" t="n">
-        <v>198.133</v>
+        <v>727</v>
       </c>
       <c r="L6" t="n">
-        <v>820.606</v>
+        <v>825</v>
       </c>
       <c r="M6" t="n">
         <v>935.616</v>
@@ -4724,13 +4724,13 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>16</v>
+        <v>170</v>
       </c>
       <c r="J7" t="n">
         <v>262.828</v>
       </c>
       <c r="K7" t="n">
-        <v>354.828</v>
+        <v>534</v>
       </c>
       <c r="L7" t="n">
         <v>626.236</v>
@@ -4792,7 +4792,7 @@
         <v>386.553</v>
       </c>
       <c r="Q8" t="n">
-        <v>478.553</v>
+        <v>541</v>
       </c>
       <c r="R8" t="n">
         <v>633</v>
@@ -4827,13 +4827,13 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>16.763</v>
+        <v>357</v>
       </c>
       <c r="I9" t="n">
         <v>450</v>
       </c>
       <c r="J9" t="n">
-        <v>558.8680000000001</v>
+        <v>652</v>
       </c>
       <c r="K9" t="n">
         <v>780.079</v>
@@ -4865,13 +4865,13 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>20</v>
+        <v>358</v>
       </c>
       <c r="I10" t="n">
         <v>453</v>
       </c>
       <c r="J10" t="n">
-        <v>561.028</v>
+        <v>665</v>
       </c>
       <c r="K10" t="n">
         <v>790.355</v>
@@ -4900,7 +4900,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>20.591</v>
+        <v>448</v>
       </c>
       <c r="H11" t="n">
         <v>570.696</v>
@@ -5057,7 +5057,7 @@
         <v>1079.777</v>
       </c>
       <c r="C1" t="n">
-        <v>4.016</v>
+        <v>15.645</v>
       </c>
     </row>
     <row r="2">
@@ -5140,10 +5140,10 @@
         <v>289.262</v>
       </c>
       <c r="AA2" t="n">
-        <v>382.868</v>
+        <v>398</v>
       </c>
       <c r="AB2" t="n">
-        <v>496.944</v>
+        <v>497</v>
       </c>
       <c r="AC2" t="n">
         <v>593.325</v>
@@ -5152,19 +5152,19 @@
         <v>685.325</v>
       </c>
       <c r="AE2" t="n">
-        <v>780.325</v>
+        <v>1346</v>
       </c>
       <c r="AF2" t="n">
-        <v>1446.77</v>
+        <v>1447</v>
       </c>
       <c r="AG2" t="n">
         <v>1545.062</v>
       </c>
       <c r="AH2" t="n">
-        <v>1642.273</v>
+        <v>1643</v>
       </c>
       <c r="AI2" t="n">
-        <v>1741</v>
+        <v>2504</v>
       </c>
       <c r="AJ2" t="n">
         <v>2601.211</v>
@@ -5205,7 +5205,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>10.77</v>
+        <v>2856</v>
       </c>
       <c r="G3" t="n">
         <v>2956.77</v>
@@ -5261,25 +5261,25 @@
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>15.133</v>
+        <v>25</v>
       </c>
       <c r="Q4" t="n">
-        <v>120.831</v>
+        <v>213</v>
       </c>
       <c r="R4" t="n">
         <v>311.602</v>
       </c>
       <c r="S4" t="n">
-        <v>409.412</v>
+        <v>1073</v>
       </c>
       <c r="T4" t="n">
         <v>1167.123</v>
       </c>
       <c r="U4" t="n">
-        <v>1260.729</v>
+        <v>1261</v>
       </c>
       <c r="V4" t="n">
-        <v>1390.051</v>
+        <v>2405</v>
       </c>
       <c r="W4" t="n">
         <v>2535.792</v>
@@ -5326,13 +5326,13 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>20.616</v>
+        <v>303</v>
       </c>
       <c r="J5" t="n">
-        <v>411.028</v>
+        <v>1253</v>
       </c>
       <c r="K5" t="n">
-        <v>1367.698</v>
+        <v>2292</v>
       </c>
       <c r="L5" t="n">
         <v>2425.738</v>
@@ -5364,7 +5364,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>22.361</v>
+        <v>2105</v>
       </c>
       <c r="H6" t="n">
         <v>2245.99</v>
@@ -5396,7 +5396,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>25.71</v>
+        <v>2009</v>
       </c>
       <c r="H7" t="n">
         <v>2159.671</v>
@@ -5428,7 +5428,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>31.048</v>
+        <v>1913</v>
       </c>
       <c r="H8" t="n">
         <v>2068.765</v>
@@ -5466,10 +5466,10 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>31.048</v>
+        <v>967</v>
       </c>
       <c r="J9" t="n">
-        <v>1069.166</v>
+        <v>1819</v>
       </c>
       <c r="K9" t="n">
         <v>1974.46</v>
@@ -5516,7 +5516,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>33.541</v>
+        <v>781</v>
       </c>
       <c r="L10" t="n">
         <v>876</v>
@@ -5531,7 +5531,7 @@
         <v>1158.831</v>
       </c>
       <c r="P10" t="n">
-        <v>1282.372</v>
+        <v>1742</v>
       </c>
       <c r="Q10" t="n">
         <v>1867.355</v>
@@ -5567,7 +5567,7 @@
         <v>1487.449</v>
       </c>
       <c r="C1" t="n">
-        <v>4.835</v>
+        <v>15.622</v>
       </c>
     </row>
     <row r="2">
@@ -5590,10 +5590,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="H2" t="n">
-        <v>57.817</v>
+        <v>161</v>
       </c>
       <c r="I2" t="n">
         <v>186.232</v>
@@ -5628,10 +5628,10 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>6.325</v>
+        <v>39</v>
       </c>
       <c r="J3" t="n">
-        <v>57.062</v>
+        <v>132</v>
       </c>
       <c r="K3" t="n">
         <v>156.142</v>
@@ -5666,10 +5666,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>11.18</v>
+        <v>99</v>
       </c>
       <c r="H4" t="n">
-        <v>116.071</v>
+        <v>159</v>
       </c>
       <c r="I4" t="n">
         <v>180.18</v>
@@ -5701,10 +5701,10 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>11.18</v>
+        <v>85</v>
       </c>
       <c r="I5" t="n">
-        <v>115.616</v>
+        <v>134</v>
       </c>
       <c r="J5" t="n">
         <v>162.028</v>
@@ -5739,13 +5739,13 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="I6" t="n">
-        <v>84.18000000000001</v>
+        <v>116</v>
       </c>
       <c r="J6" t="n">
-        <v>140.142</v>
+        <v>153</v>
       </c>
       <c r="K6" t="n">
         <v>193</v>
@@ -5774,10 +5774,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>15.811</v>
+        <v>87</v>
       </c>
       <c r="H7" t="n">
-        <v>110.892</v>
+        <v>165</v>
       </c>
       <c r="I7" t="n">
         <v>202.803</v>
@@ -5803,7 +5803,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>16.971</v>
+        <v>124</v>
       </c>
       <c r="G8" t="n">
         <v>150.971</v>
@@ -5835,10 +5835,10 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>17.464</v>
+        <v>50</v>
       </c>
       <c r="I9" t="n">
-        <v>68.062</v>
+        <v>124</v>
       </c>
       <c r="J9" t="n">
         <v>144.296</v>
@@ -5876,16 +5876,16 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="J10" t="n">
         <v>70.44</v>
       </c>
       <c r="K10" t="n">
-        <v>90.44</v>
+        <v>97</v>
       </c>
       <c r="L10" t="n">
-        <v>130.087</v>
+        <v>132</v>
       </c>
       <c r="M10" t="n">
         <v>176.176</v>
@@ -5917,13 +5917,13 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>20.616</v>
+        <v>34</v>
       </c>
       <c r="I11" t="n">
-        <v>55.18</v>
+        <v>75</v>
       </c>
       <c r="J11" t="n">
-        <v>114.12</v>
+        <v>117</v>
       </c>
       <c r="K11" t="n">
         <v>162.468</v>
@@ -5952,7 +5952,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>21.213</v>
+        <v>81</v>
       </c>
       <c r="H12" t="n">
         <v>103.207</v>
@@ -5987,13 +5987,13 @@
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>24.759</v>
+        <v>37</v>
       </c>
       <c r="I13" t="n">
-        <v>55.246</v>
+        <v>97</v>
       </c>
       <c r="J13" t="n">
-        <v>116.434</v>
+        <v>143</v>
       </c>
       <c r="K13" t="n">
         <v>194.037</v>
@@ -6022,10 +6022,10 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>25.495</v>
+        <v>71</v>
       </c>
       <c r="H14" t="n">
-        <v>88.071</v>
+        <v>126</v>
       </c>
       <c r="I14" t="n">
         <v>167.623</v>
@@ -6057,13 +6057,13 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>25.495</v>
+        <v>31</v>
       </c>
       <c r="I15" t="n">
-        <v>50.22</v>
+        <v>61</v>
       </c>
       <c r="J15" t="n">
-        <v>83.166</v>
+        <v>97</v>
       </c>
       <c r="K15" t="n">
         <v>135.862</v>
@@ -6098,7 +6098,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>29.155</v>
+        <v>32</v>
       </c>
       <c r="J16" t="n">
         <v>60.111</v>
@@ -6107,7 +6107,7 @@
         <v>78.173</v>
       </c>
       <c r="L16" t="n">
-        <v>100.215</v>
+        <v>108</v>
       </c>
       <c r="M16" t="n">
         <v>161.932</v>
@@ -6136,10 +6136,10 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>29.833</v>
+        <v>63</v>
       </c>
       <c r="H17" t="n">
-        <v>86.038</v>
+        <v>117</v>
       </c>
       <c r="I17" t="n">
         <v>163.056</v>
@@ -6168,7 +6168,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>31.89</v>
+        <v>69</v>
       </c>
       <c r="H18" t="n">
         <v>89.81699999999999</v>
@@ -6223,7 +6223,7 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>33.541</v>
+        <v>67</v>
       </c>
       <c r="G20" t="n">
         <v>110.541</v>
@@ -6252,10 +6252,10 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>33.971</v>
+        <v>44</v>
       </c>
       <c r="H21" t="n">
-        <v>62.602</v>
+        <v>68</v>
       </c>
       <c r="I21" t="n">
         <v>114.056</v>
@@ -6317,7 +6317,7 @@
         <v>370.233</v>
       </c>
       <c r="C1" t="n">
-        <v>1.2</v>
+        <v>15.929</v>
       </c>
     </row>
     <row r="2">
@@ -6343,7 +6343,7 @@
         <v>10</v>
       </c>
       <c r="H2" t="n">
-        <v>102</v>
+        <v>914</v>
       </c>
       <c r="I2" t="n">
         <v>1014.198</v>
@@ -6372,7 +6372,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>12.166</v>
+        <v>812</v>
       </c>
       <c r="H3" t="n">
         <v>925.345</v>
@@ -6404,7 +6404,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>13</v>
+        <v>732</v>
       </c>
       <c r="H4" t="n">
         <v>844.672</v>
@@ -6451,13 +6451,13 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="M5" t="n">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="N5" t="n">
-        <v>276.205</v>
+        <v>357</v>
       </c>
       <c r="O5" t="n">
         <v>450</v>
@@ -6519,7 +6519,7 @@
         <v>290.961</v>
       </c>
       <c r="N6" t="n">
-        <v>402.362</v>
+        <v>652</v>
       </c>
       <c r="O6" t="n">
         <v>780.079</v>
@@ -6617,7 +6617,7 @@
         <v>1218.356</v>
       </c>
       <c r="C1" t="n">
-        <v>3.366</v>
+        <v>14.562</v>
       </c>
     </row>
     <row r="2">
@@ -6652,19 +6652,19 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="L2" t="n">
         <v>120.708</v>
       </c>
       <c r="M2" t="n">
-        <v>138.77</v>
+        <v>588</v>
       </c>
       <c r="N2" t="n">
-        <v>612.1420000000001</v>
+        <v>678</v>
       </c>
       <c r="O2" t="n">
-        <v>698</v>
+        <v>817</v>
       </c>
       <c r="P2" t="n">
         <v>842</v>
@@ -6705,16 +6705,16 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>11.18</v>
+        <v>415</v>
       </c>
       <c r="K3" t="n">
-        <v>432.071</v>
+        <v>690</v>
       </c>
       <c r="L3" t="n">
-        <v>725.495</v>
+        <v>733</v>
       </c>
       <c r="M3" t="n">
-        <v>766.409</v>
+        <v>773</v>
       </c>
       <c r="N3" t="n">
         <v>811.16</v>
@@ -6761,16 +6761,16 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>11.18</v>
+        <v>360</v>
       </c>
       <c r="M4" t="n">
-        <v>385.811</v>
+        <v>409</v>
       </c>
       <c r="N4" t="n">
         <v>423.243</v>
       </c>
       <c r="O4" t="n">
-        <v>452.659</v>
+        <v>620</v>
       </c>
       <c r="P4" t="n">
         <v>647.263</v>
@@ -6817,16 +6817,16 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>15</v>
+        <v>228</v>
       </c>
       <c r="K5" t="n">
-        <v>249.18</v>
+        <v>527</v>
       </c>
       <c r="L5" t="n">
-        <v>545.246</v>
+        <v>547</v>
       </c>
       <c r="M5" t="n">
-        <v>575.111</v>
+        <v>581</v>
       </c>
       <c r="N5" t="n">
         <v>606.811</v>
@@ -6867,7 +6867,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>15.811</v>
+        <v>377</v>
       </c>
       <c r="K6" t="n">
         <v>397</v>
@@ -6876,7 +6876,7 @@
         <v>419.207</v>
       </c>
       <c r="M6" t="n">
-        <v>438.641</v>
+        <v>515</v>
       </c>
       <c r="N6" t="n">
         <v>588.388</v>
@@ -6914,16 +6914,16 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>17.464</v>
+        <v>152</v>
       </c>
       <c r="J7" t="n">
-        <v>174.042</v>
+        <v>259</v>
       </c>
       <c r="K7" t="n">
-        <v>284</v>
+        <v>400</v>
       </c>
       <c r="L7" t="n">
-        <v>459.649</v>
+        <v>501</v>
       </c>
       <c r="M7" t="n">
         <v>554.932</v>
@@ -6967,10 +6967,10 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>18</v>
+        <v>143</v>
       </c>
       <c r="M8" t="n">
-        <v>163.44</v>
+        <v>214</v>
       </c>
       <c r="N8" t="n">
         <v>242.028</v>
@@ -7026,19 +7026,19 @@
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>20.616</v>
+        <v>34</v>
       </c>
       <c r="L9" t="n">
         <v>56.042</v>
       </c>
       <c r="M9" t="n">
-        <v>84.15300000000001</v>
+        <v>85</v>
       </c>
       <c r="N9" t="n">
         <v>102.211</v>
       </c>
       <c r="O9" t="n">
-        <v>125.211</v>
+        <v>269</v>
       </c>
       <c r="P9" t="n">
         <v>286.071</v>
@@ -7070,10 +7070,10 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>24.759</v>
+        <v>45</v>
       </c>
       <c r="H10" t="n">
-        <v>69.866</v>
+        <v>190</v>
       </c>
       <c r="I10" t="n">
         <v>229.833</v>
@@ -7147,7 +7147,7 @@
         <v>1635.534</v>
       </c>
       <c r="C1" t="n">
-        <v>5.627</v>
+        <v>16.59</v>
       </c>
     </row>
     <row r="2">
@@ -7182,10 +7182,10 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>30.806</v>
+        <v>50</v>
       </c>
       <c r="L2" t="n">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="M2" t="n">
         <v>108</v>
@@ -7194,7 +7194,7 @@
         <v>123.831</v>
       </c>
       <c r="O2" t="n">
-        <v>135.831</v>
+        <v>141</v>
       </c>
       <c r="P2" t="n">
         <v>158.071</v>
@@ -7229,13 +7229,13 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>30.806</v>
+        <v>92</v>
       </c>
       <c r="I3" t="n">
-        <v>111.899</v>
+        <v>124</v>
       </c>
       <c r="J3" t="n">
-        <v>137.606</v>
+        <v>139</v>
       </c>
       <c r="K3" t="n">
         <v>193.204</v>
@@ -7267,10 +7267,10 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>31.623</v>
+        <v>119</v>
       </c>
       <c r="I4" t="n">
-        <v>136.071</v>
+        <v>142</v>
       </c>
       <c r="J4" t="n">
         <v>163.18</v>
@@ -7311,7 +7311,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>32.388</v>
+        <v>64</v>
       </c>
       <c r="K5" t="n">
         <v>79</v>
@@ -7320,7 +7320,7 @@
         <v>94.38500000000001</v>
       </c>
       <c r="M5" t="n">
-        <v>138.794</v>
+        <v>148</v>
       </c>
       <c r="N5" t="n">
         <v>168.44</v>
@@ -7358,10 +7358,10 @@
         <v>33.541</v>
       </c>
       <c r="I6" t="n">
-        <v>45.541</v>
+        <v>64</v>
       </c>
       <c r="J6" t="n">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="K6" t="n">
         <v>176.079</v>
@@ -7393,13 +7393,13 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="I7" t="n">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="J7" t="n">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="K7" t="n">
         <v>206.044</v>
@@ -7431,7 +7431,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>35.341</v>
+        <v>116</v>
       </c>
       <c r="I8" t="n">
         <v>139</v>
@@ -7519,10 +7519,10 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>36.056</v>
+        <v>37</v>
       </c>
       <c r="I10" t="n">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="J10" t="n">
         <v>90.38500000000001</v>
@@ -7563,7 +7563,7 @@
         <v>50.736</v>
       </c>
       <c r="J11" t="n">
-        <v>67.807</v>
+        <v>91</v>
       </c>
       <c r="K11" t="n">
         <v>140.051</v>
@@ -7589,7 +7589,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>38.053</v>
+        <v>104</v>
       </c>
       <c r="G12" t="n">
         <v>152.053</v>
@@ -7618,7 +7618,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>40.05</v>
+        <v>72</v>
       </c>
       <c r="H13" t="n">
         <v>87.38500000000001</v>
@@ -7682,7 +7682,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="H15" t="n">
         <v>79</v>
@@ -7717,7 +7717,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>50.289</v>
+        <v>61</v>
       </c>
       <c r="I16" t="n">
         <v>73</v>
@@ -7758,7 +7758,7 @@
         <v>51.478</v>
       </c>
       <c r="I17" t="n">
-        <v>67.309</v>
+        <v>74</v>
       </c>
       <c r="J17" t="n">
         <v>88</v>
@@ -7797,7 +7797,7 @@
         <v>1630.627</v>
       </c>
       <c r="C1" t="n">
-        <v>3.251</v>
+        <v>31.261</v>
       </c>
     </row>
     <row r="2">
@@ -7844,10 +7844,10 @@
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>30.806</v>
+        <v>152</v>
       </c>
       <c r="P2" t="n">
-        <v>166</v>
+        <v>388</v>
       </c>
       <c r="Q2" t="n">
         <v>401</v>
@@ -7856,13 +7856,13 @@
         <v>416</v>
       </c>
       <c r="S2" t="n">
-        <v>429</v>
+        <v>489</v>
       </c>
       <c r="T2" t="n">
-        <v>501</v>
+        <v>644</v>
       </c>
       <c r="U2" t="n">
-        <v>661.071</v>
+        <v>673</v>
       </c>
       <c r="V2" t="n">
         <v>725</v>
@@ -7915,13 +7915,13 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>30.806</v>
+        <v>376</v>
       </c>
       <c r="M3" t="n">
         <v>392.403</v>
       </c>
       <c r="N3" t="n">
-        <v>406.009</v>
+        <v>557</v>
       </c>
       <c r="O3" t="n">
         <v>577.4400000000001</v>
@@ -7962,10 +7962,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>31.623</v>
+        <v>519</v>
       </c>
       <c r="H4" t="n">
-        <v>536.071</v>
+        <v>653</v>
       </c>
       <c r="I4" t="n">
         <v>701.079</v>
@@ -8012,19 +8012,19 @@
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>32.388</v>
+        <v>223</v>
       </c>
       <c r="N5" t="n">
         <v>238</v>
       </c>
       <c r="O5" t="n">
-        <v>253.385</v>
+        <v>371</v>
       </c>
       <c r="P5" t="n">
         <v>417.056</v>
       </c>
       <c r="Q5" t="n">
-        <v>429.056</v>
+        <v>537</v>
       </c>
       <c r="R5" t="n">
         <v>550</v>
@@ -8074,13 +8074,13 @@
         <v>33.541</v>
       </c>
       <c r="K6" t="n">
-        <v>45.541</v>
+        <v>217</v>
       </c>
       <c r="L6" t="n">
-        <v>232.831</v>
+        <v>329</v>
       </c>
       <c r="M6" t="n">
-        <v>377</v>
+        <v>471</v>
       </c>
       <c r="N6" t="n">
         <v>561.4299999999999</v>
@@ -8127,19 +8127,19 @@
         <v>35.355</v>
       </c>
       <c r="L7" t="n">
-        <v>48.355</v>
+        <v>105</v>
       </c>
       <c r="M7" t="n">
-        <v>120</v>
+        <v>174</v>
       </c>
       <c r="N7" t="n">
-        <v>186</v>
+        <v>255</v>
       </c>
       <c r="O7" t="n">
         <v>316.614</v>
       </c>
       <c r="P7" t="n">
-        <v>331.999</v>
+        <v>335</v>
       </c>
       <c r="Q7" t="n">
         <v>390.177</v>
@@ -8183,7 +8183,7 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>36.056</v>
+        <v>64</v>
       </c>
       <c r="M8" t="n">
         <v>81.071</v>
@@ -8236,10 +8236,10 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>50.289</v>
+        <v>165</v>
       </c>
       <c r="J9" t="n">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="K9" t="n">
         <v>209</v>
@@ -8271,7 +8271,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>51.478</v>
+        <v>80</v>
       </c>
       <c r="G10" t="n">
         <v>141.478</v>
@@ -8307,7 +8307,7 @@
         <v>1870.696</v>
       </c>
       <c r="C1" t="n">
-        <v>13.171</v>
+        <v>39.621</v>
       </c>
     </row>
     <row r="2">
@@ -8336,10 +8336,10 @@
         <v>10</v>
       </c>
       <c r="I2" t="n">
-        <v>102</v>
+        <v>914</v>
       </c>
       <c r="J2" t="n">
-        <v>1021</v>
+        <v>1054</v>
       </c>
       <c r="K2" t="n">
         <v>1162.028</v>
@@ -8368,10 +8368,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>12.166</v>
+        <v>812</v>
       </c>
       <c r="H3" t="n">
-        <v>919</v>
+        <v>1001</v>
       </c>
       <c r="I3" t="n">
         <v>1110.209</v>
@@ -8427,7 +8427,7 @@
         <v>290.207</v>
       </c>
       <c r="P4" t="n">
-        <v>383.207</v>
+        <v>826</v>
       </c>
       <c r="Q4" t="n">
         <v>918</v>
@@ -8462,10 +8462,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>13</v>
+        <v>732</v>
       </c>
       <c r="H5" t="n">
-        <v>842.224</v>
+        <v>912</v>
       </c>
       <c r="I5" t="n">
         <v>1023.213</v>
@@ -8509,22 +8509,22 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="M6" t="n">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="N6" t="n">
         <v>261</v>
       </c>
       <c r="O6" t="n">
-        <v>354</v>
+        <v>546</v>
       </c>
       <c r="P6" t="n">
         <v>638</v>
       </c>
       <c r="Q6" t="n">
-        <v>747.723</v>
+        <v>751</v>
       </c>
       <c r="R6" t="n">
         <v>863.204</v>
@@ -8568,10 +8568,10 @@
         <v>106.133</v>
       </c>
       <c r="K7" t="n">
-        <v>198.133</v>
+        <v>727</v>
       </c>
       <c r="L7" t="n">
-        <v>820</v>
+        <v>912</v>
       </c>
       <c r="M7" t="n">
         <v>1020.682</v>
@@ -8609,19 +8609,19 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>16</v>
+        <v>170</v>
       </c>
       <c r="K8" t="n">
         <v>262.828</v>
       </c>
       <c r="L8" t="n">
-        <v>354.828</v>
+        <v>534</v>
       </c>
       <c r="M8" t="n">
         <v>626.236</v>
       </c>
       <c r="N8" t="n">
-        <v>721.335</v>
+        <v>825</v>
       </c>
       <c r="O8" t="n">
         <v>935.616</v>
@@ -8686,7 +8686,7 @@
         <v>386.553</v>
       </c>
       <c r="S9" t="n">
-        <v>478.553</v>
+        <v>541</v>
       </c>
       <c r="T9" t="n">
         <v>633</v>
@@ -8730,13 +8730,13 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>16.763</v>
+        <v>357</v>
       </c>
       <c r="J10" t="n">
         <v>450</v>
       </c>
       <c r="K10" t="n">
-        <v>558.8680000000001</v>
+        <v>652</v>
       </c>
       <c r="L10" t="n">
         <v>772.414</v>
@@ -8777,10 +8777,10 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>19.849</v>
+        <v>353</v>
       </c>
       <c r="K11" t="n">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="L11" t="n">
         <v>543</v>
@@ -8789,7 +8789,7 @@
         <v>635</v>
       </c>
       <c r="N11" t="n">
-        <v>728</v>
+        <v>734</v>
       </c>
       <c r="O11" t="n">
         <v>844.616</v>
@@ -8821,13 +8821,13 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>20</v>
+        <v>358</v>
       </c>
       <c r="I12" t="n">
         <v>453</v>
       </c>
       <c r="J12" t="n">
-        <v>561.028</v>
+        <v>665</v>
       </c>
       <c r="K12" t="n">
         <v>790.355</v>
@@ -8859,10 +8859,10 @@
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>20.591</v>
+        <v>448</v>
       </c>
       <c r="I13" t="n">
-        <v>556.788</v>
+        <v>651</v>
       </c>
       <c r="J13" t="n">
         <v>789.052</v>
@@ -8897,7 +8897,7 @@
         <v>20.616</v>
       </c>
       <c r="H14" t="n">
-        <v>114.859</v>
+        <v>737</v>
       </c>
       <c r="I14" t="n">
         <v>851.352</v>
@@ -8935,16 +8935,16 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>25.495</v>
+        <v>85</v>
       </c>
       <c r="K15" t="n">
         <v>176</v>
       </c>
       <c r="L15" t="n">
-        <v>271</v>
+        <v>458</v>
       </c>
       <c r="M15" t="n">
-        <v>550.828</v>
+        <v>555</v>
       </c>
       <c r="N15" t="n">
         <v>648</v>
@@ -9071,7 +9071,7 @@
         <v>311.797</v>
       </c>
       <c r="P17" t="n">
-        <v>404.797</v>
+        <v>475</v>
       </c>
       <c r="Q17" t="n">
         <v>570</v>
@@ -9171,13 +9171,13 @@
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>32.388</v>
+        <v>265</v>
       </c>
       <c r="I19" t="n">
-        <v>358</v>
+        <v>369</v>
       </c>
       <c r="J19" t="n">
-        <v>487.178</v>
+        <v>574</v>
       </c>
       <c r="K19" t="n">
         <v>716</v>
@@ -9268,7 +9268,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>44.204</v>
+        <v>368</v>
       </c>
       <c r="H21" t="n">
         <v>518.415</v>
@@ -9357,7 +9357,7 @@
         <v>1880.467</v>
       </c>
       <c r="C1" t="n">
-        <v>14.007</v>
+        <v>31.108</v>
       </c>
     </row>
     <row r="2">
@@ -9464,10 +9464,10 @@
         <v>677.679</v>
       </c>
       <c r="AI2" t="n">
-        <v>773.064</v>
+        <v>881</v>
       </c>
       <c r="AJ2" t="n">
-        <v>977.403</v>
+        <v>978</v>
       </c>
       <c r="AK2" t="n">
         <v>1073</v>
@@ -9476,7 +9476,7 @@
         <v>1167.123</v>
       </c>
       <c r="AM2" t="n">
-        <v>1260.729</v>
+        <v>1261</v>
       </c>
       <c r="AN2" t="n">
         <v>1355.472</v>
@@ -9488,7 +9488,7 @@
         <v>1546.129</v>
       </c>
       <c r="AQ2" t="n">
-        <v>1641.228</v>
+        <v>1736</v>
       </c>
       <c r="AR2" t="n">
         <v>1832</v>
@@ -9497,10 +9497,10 @@
         <v>1925</v>
       </c>
       <c r="AT2" t="n">
-        <v>2025.44</v>
+        <v>2900</v>
       </c>
       <c r="AU2" t="n">
-        <v>2998.062</v>
+        <v>3097</v>
       </c>
       <c r="AV2" t="n">
         <v>3196.849</v>
@@ -9595,10 +9595,10 @@
         <v>289.262</v>
       </c>
       <c r="AB3" t="n">
-        <v>382.868</v>
+        <v>398</v>
       </c>
       <c r="AC3" t="n">
-        <v>496.944</v>
+        <v>497</v>
       </c>
       <c r="AD3" t="n">
         <v>593.325</v>
@@ -9607,19 +9607,19 @@
         <v>685.325</v>
       </c>
       <c r="AF3" t="n">
-        <v>780.325</v>
+        <v>1346</v>
       </c>
       <c r="AG3" t="n">
-        <v>1446.77</v>
+        <v>1447</v>
       </c>
       <c r="AH3" t="n">
         <v>1545.062</v>
       </c>
       <c r="AI3" t="n">
-        <v>1642.273</v>
+        <v>1643</v>
       </c>
       <c r="AJ3" t="n">
-        <v>1741</v>
+        <v>2504</v>
       </c>
       <c r="AK3" t="n">
         <v>2601.211</v>
@@ -9663,7 +9663,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>10.77</v>
+        <v>2856</v>
       </c>
       <c r="G4" t="n">
         <v>2956.77</v>
@@ -9746,13 +9746,13 @@
         <v>200.207</v>
       </c>
       <c r="Y5" t="n">
-        <v>293.207</v>
+        <v>588</v>
       </c>
       <c r="Z5" t="n">
         <v>680</v>
       </c>
       <c r="AA5" t="n">
-        <v>775.831</v>
+        <v>776</v>
       </c>
       <c r="AB5" t="n">
         <v>871.385</v>
@@ -9764,22 +9764,22 @@
         <v>1065.598</v>
       </c>
       <c r="AE5" t="n">
-        <v>1159.598</v>
+        <v>1725</v>
       </c>
       <c r="AF5" t="n">
-        <v>1818.606</v>
+        <v>1819</v>
       </c>
       <c r="AG5" t="n">
         <v>1913.472</v>
       </c>
       <c r="AH5" t="n">
-        <v>2008.857</v>
+        <v>2009</v>
       </c>
       <c r="AI5" t="n">
         <v>2105.403</v>
       </c>
       <c r="AJ5" t="n">
-        <v>2199.009</v>
+        <v>2666</v>
       </c>
       <c r="AK5" t="n">
         <v>2758</v>
@@ -9814,7 +9814,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>16.553</v>
+        <v>2573</v>
       </c>
       <c r="H6" t="n">
         <v>2715</v>
@@ -9849,7 +9849,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>18.028</v>
+        <v>2480</v>
       </c>
       <c r="I7" t="n">
         <v>2625.902</v>
@@ -9908,7 +9908,7 @@
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>19.849</v>
+        <v>213</v>
       </c>
       <c r="P8" t="n">
         <v>308</v>
@@ -9920,13 +9920,13 @@
         <v>493</v>
       </c>
       <c r="S8" t="n">
-        <v>603.881</v>
+        <v>1160</v>
       </c>
       <c r="T8" t="n">
-        <v>1254</v>
+        <v>1630</v>
       </c>
       <c r="U8" t="n">
-        <v>1743.854</v>
+        <v>2200</v>
       </c>
       <c r="V8" t="n">
         <v>2292.236</v>
@@ -9973,16 +9973,16 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>20.616</v>
+        <v>303</v>
       </c>
       <c r="K9" t="n">
-        <v>411.028</v>
+        <v>1253</v>
       </c>
       <c r="L9" t="n">
-        <v>1374.623</v>
+        <v>1742</v>
       </c>
       <c r="M9" t="n">
-        <v>1835</v>
+        <v>2311</v>
       </c>
       <c r="N9" t="n">
         <v>2487.608</v>
@@ -10023,13 +10023,13 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>31.048</v>
+        <v>1641</v>
       </c>
       <c r="K10" t="n">
-        <v>1751</v>
+        <v>2029</v>
       </c>
       <c r="L10" t="n">
-        <v>2130.705</v>
+        <v>2131</v>
       </c>
       <c r="M10" t="n">
         <v>2226</v>
@@ -10079,7 +10079,7 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>33.541</v>
+        <v>781</v>
       </c>
       <c r="M11" t="n">
         <v>876</v>
@@ -10094,10 +10094,10 @@
         <v>1158.831</v>
       </c>
       <c r="Q11" t="n">
-        <v>1286.91</v>
+        <v>1837</v>
       </c>
       <c r="R11" t="n">
-        <v>1932</v>
+        <v>2216</v>
       </c>
       <c r="S11" t="n">
         <v>2342.056</v>
@@ -10123,7 +10123,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>38.079</v>
+        <v>2119</v>
       </c>
       <c r="G12" t="n">
         <v>2247.079</v>
@@ -10149,7 +10149,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>39.357</v>
+        <v>2026</v>
       </c>
       <c r="G13" t="n">
         <v>2155.357</v>
@@ -10175,7 +10175,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>40.311</v>
+        <v>1934</v>
       </c>
       <c r="G14" t="n">
         <v>2064.311</v>
@@ -10213,10 +10213,10 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>40.608</v>
+        <v>788</v>
       </c>
       <c r="K15" t="n">
-        <v>957.812</v>
+        <v>1256</v>
       </c>
       <c r="L15" t="n">
         <v>1350</v>
@@ -10251,7 +10251,7 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>44.204</v>
+        <v>694</v>
       </c>
       <c r="G16" t="n">
         <v>828.204</v>
@@ -10287,7 +10287,7 @@
         <v>2623.247</v>
       </c>
       <c r="C1" t="n">
-        <v>14.354</v>
+        <v>33.747</v>
       </c>
     </row>
     <row r="2">
@@ -10310,10 +10310,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>4.472</v>
+        <v>95</v>
       </c>
       <c r="H2" t="n">
-        <v>110.099</v>
+        <v>200</v>
       </c>
       <c r="I2" t="n">
         <v>219.055</v>
@@ -10348,16 +10348,16 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="J3" t="n">
         <v>54.28</v>
       </c>
       <c r="K3" t="n">
-        <v>68.752</v>
+        <v>161</v>
       </c>
       <c r="L3" t="n">
-        <v>179.062</v>
+        <v>182</v>
       </c>
       <c r="M3" t="n">
         <v>213.095</v>
@@ -10389,13 +10389,13 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>6.325</v>
+        <v>39</v>
       </c>
       <c r="I4" t="n">
-        <v>57.062</v>
+        <v>132</v>
       </c>
       <c r="J4" t="n">
-        <v>155.038</v>
+        <v>182</v>
       </c>
       <c r="K4" t="n">
         <v>213.095</v>
@@ -10421,7 +10421,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>9</v>
+        <v>176</v>
       </c>
       <c r="G5" t="n">
         <v>195</v>
@@ -10453,13 +10453,13 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>11.18</v>
+        <v>99</v>
       </c>
       <c r="I6" t="n">
-        <v>113.243</v>
+        <v>135</v>
       </c>
       <c r="J6" t="n">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="K6" t="n">
         <v>218.248</v>
@@ -10488,10 +10488,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>11.18</v>
+        <v>159</v>
       </c>
       <c r="H7" t="n">
-        <v>182.892</v>
+        <v>185</v>
       </c>
       <c r="I7" t="n">
         <v>219.042</v>
@@ -10523,10 +10523,10 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>11.18</v>
+        <v>85</v>
       </c>
       <c r="I8" t="n">
-        <v>108.416</v>
+        <v>149</v>
       </c>
       <c r="J8" t="n">
         <v>179.248</v>
@@ -10561,13 +10561,13 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>11.314</v>
+        <v>52</v>
       </c>
       <c r="I9" t="n">
-        <v>69.616</v>
+        <v>87</v>
       </c>
       <c r="J9" t="n">
-        <v>103.708</v>
+        <v>162</v>
       </c>
       <c r="K9" t="n">
         <v>190.028</v>
@@ -10599,13 +10599,13 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>12.042</v>
+        <v>100</v>
       </c>
       <c r="I10" t="n">
-        <v>116.083</v>
+        <v>133</v>
       </c>
       <c r="J10" t="n">
-        <v>153.198</v>
+        <v>160</v>
       </c>
       <c r="K10" t="n">
         <v>195.612</v>
@@ -10643,16 +10643,16 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>14.866</v>
+        <v>39</v>
       </c>
       <c r="K11" t="n">
-        <v>54.385</v>
+        <v>83</v>
       </c>
       <c r="L11" t="n">
         <v>98.657</v>
       </c>
       <c r="M11" t="n">
-        <v>113.129</v>
+        <v>134</v>
       </c>
       <c r="N11" t="n">
         <v>162.028</v>
@@ -10687,13 +10687,13 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="I12" t="n">
         <v>80.071</v>
       </c>
       <c r="J12" t="n">
-        <v>94.194</v>
+        <v>179</v>
       </c>
       <c r="K12" t="n">
         <v>208.698</v>
@@ -10722,7 +10722,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>16.971</v>
+        <v>124</v>
       </c>
       <c r="H13" t="n">
         <v>146.042</v>
@@ -10760,16 +10760,16 @@
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>17.464</v>
+        <v>50</v>
       </c>
       <c r="J14" t="n">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="K14" t="n">
         <v>90.325</v>
       </c>
       <c r="L14" t="n">
-        <v>107.605</v>
+        <v>165</v>
       </c>
       <c r="M14" t="n">
         <v>202.803</v>
@@ -10807,16 +10807,16 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>17.804</v>
+        <v>18</v>
       </c>
       <c r="K15" t="n">
-        <v>31.606</v>
+        <v>58</v>
       </c>
       <c r="L15" t="n">
-        <v>75.616</v>
+        <v>76</v>
       </c>
       <c r="M15" t="n">
-        <v>93.071</v>
+        <v>101</v>
       </c>
       <c r="N15" t="n">
         <v>141.463</v>
@@ -10854,10 +10854,10 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="J16" t="n">
-        <v>65.831</v>
+        <v>101</v>
       </c>
       <c r="K16" t="n">
         <v>132</v>
@@ -10901,16 +10901,16 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>18.028</v>
+        <v>62</v>
       </c>
       <c r="K17" t="n">
-        <v>75.16200000000001</v>
+        <v>78</v>
       </c>
       <c r="L17" t="n">
-        <v>95.071</v>
+        <v>97</v>
       </c>
       <c r="M17" t="n">
-        <v>129.204</v>
+        <v>136</v>
       </c>
       <c r="N17" t="n">
         <v>158.166</v>
@@ -10942,10 +10942,10 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>18.385</v>
+        <v>93</v>
       </c>
       <c r="H18" t="n">
-        <v>134.016</v>
+        <v>140</v>
       </c>
       <c r="I18" t="n">
         <v>172.804</v>
@@ -10986,10 +10986,10 @@
         <v>38.583</v>
       </c>
       <c r="K19" t="n">
-        <v>57.803</v>
+        <v>61</v>
       </c>
       <c r="L19" t="n">
-        <v>83.166</v>
+        <v>97</v>
       </c>
       <c r="M19" t="n">
         <v>135.862</v>
@@ -11024,16 +11024,16 @@
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>20.616</v>
+        <v>34</v>
       </c>
       <c r="J20" t="n">
         <v>51.071</v>
       </c>
       <c r="K20" t="n">
-        <v>68.282</v>
+        <v>95</v>
       </c>
       <c r="L20" t="n">
-        <v>114.434</v>
+        <v>117</v>
       </c>
       <c r="M20" t="n">
         <v>162.468</v>
@@ -11062,7 +11062,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>22.361</v>
+        <v>116</v>
       </c>
       <c r="H21" t="n">
         <v>147.541</v>
@@ -11097,10 +11097,10 @@
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>22.472</v>
+        <v>35</v>
       </c>
       <c r="I22" t="n">
-        <v>50.385</v>
+        <v>69</v>
       </c>
       <c r="J22" t="n">
         <v>125.819</v>
@@ -11138,13 +11138,13 @@
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>23.324</v>
+        <v>55</v>
       </c>
       <c r="J23" t="n">
         <v>78</v>
       </c>
       <c r="K23" t="n">
-        <v>100.042</v>
+        <v>108</v>
       </c>
       <c r="L23" t="n">
         <v>147.017</v>
@@ -11179,13 +11179,13 @@
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>24.759</v>
+        <v>37</v>
       </c>
       <c r="I24" t="n">
-        <v>49.828</v>
+        <v>94</v>
       </c>
       <c r="J24" t="n">
-        <v>118.866</v>
+        <v>126</v>
       </c>
       <c r="K24" t="n">
         <v>167.623</v>
@@ -11211,7 +11211,7 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>25.495</v>
+        <v>124</v>
       </c>
       <c r="G25" t="n">
         <v>159.495</v>
@@ -11246,7 +11246,7 @@
         <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>25.495</v>
+        <v>71</v>
       </c>
       <c r="J26" t="n">
         <v>90.22</v>
@@ -11287,7 +11287,7 @@
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>25.495</v>
+        <v>58</v>
       </c>
       <c r="I27" t="n">
         <v>76.062</v>
@@ -11319,7 +11319,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>25.554</v>
+        <v>92</v>
       </c>
       <c r="G28" t="n">
         <v>127.554</v>
@@ -11348,10 +11348,10 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>29.155</v>
+        <v>75</v>
       </c>
       <c r="H29" t="n">
-        <v>91.325</v>
+        <v>94</v>
       </c>
       <c r="I29" t="n">
         <v>139.355</v>
@@ -11380,7 +11380,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>29.155</v>
+        <v>32</v>
       </c>
       <c r="H30" t="n">
         <v>60.111</v>
@@ -11412,10 +11412,10 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>29.833</v>
+        <v>63</v>
       </c>
       <c r="H31" t="n">
-        <v>83.44</v>
+        <v>96</v>
       </c>
       <c r="I31" t="n">
         <v>137.064</v>
@@ -11444,7 +11444,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>31.89</v>
+        <v>69</v>
       </c>
       <c r="H32" t="n">
         <v>89.81699999999999</v>
@@ -11505,10 +11505,10 @@
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>33.971</v>
+        <v>44</v>
       </c>
       <c r="I34" t="n">
-        <v>62.602</v>
+        <v>68</v>
       </c>
       <c r="J34" t="n">
         <v>90</v>
@@ -11543,7 +11543,7 @@
         <v>34.928</v>
       </c>
       <c r="H35" t="n">
-        <v>59.35</v>
+        <v>73</v>
       </c>
       <c r="I35" t="n">
         <v>129.519</v>
@@ -11569,7 +11569,7 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>39.661</v>
+        <v>77</v>
       </c>
       <c r="G36" t="n">
         <v>126.661</v>
@@ -11621,7 +11621,7 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>49.93</v>
+        <v>51</v>
       </c>
       <c r="G38" t="n">
         <v>110.93</v>
@@ -11657,7 +11657,7 @@
         <v>1984.957</v>
       </c>
       <c r="C1" t="n">
-        <v>12.154</v>
+        <v>30.019</v>
       </c>
     </row>
     <row r="2">
@@ -11692,10 +11692,10 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>4.472</v>
+        <v>414</v>
       </c>
       <c r="L2" t="n">
-        <v>429.099</v>
+        <v>849</v>
       </c>
       <c r="M2" t="n">
         <v>872.454</v>
@@ -11751,19 +11751,19 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="M3" t="n">
         <v>120.708</v>
       </c>
       <c r="N3" t="n">
-        <v>138.77</v>
+        <v>588</v>
       </c>
       <c r="O3" t="n">
-        <v>610.042</v>
+        <v>641</v>
       </c>
       <c r="P3" t="n">
-        <v>659.062</v>
+        <v>839</v>
       </c>
       <c r="Q3" t="n">
         <v>855.708</v>
@@ -11822,13 +11822,13 @@
         <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>11.18</v>
+        <v>415</v>
       </c>
       <c r="P4" t="n">
-        <v>428.162</v>
+        <v>436</v>
       </c>
       <c r="Q4" t="n">
-        <v>450</v>
+        <v>607</v>
       </c>
       <c r="R4" t="n">
         <v>623.708</v>
@@ -11837,7 +11837,7 @@
         <v>638.807</v>
       </c>
       <c r="T4" t="n">
-        <v>653.9059999999999</v>
+        <v>739</v>
       </c>
       <c r="U4" t="n">
         <v>763.866</v>
@@ -11893,13 +11893,13 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>11.18</v>
+        <v>360</v>
       </c>
       <c r="M5" t="n">
         <v>378.944</v>
       </c>
       <c r="N5" t="n">
-        <v>393.416</v>
+        <v>681</v>
       </c>
       <c r="O5" t="n">
         <v>702.402</v>
@@ -11964,10 +11964,10 @@
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>11.314</v>
+        <v>174</v>
       </c>
       <c r="P6" t="n">
-        <v>191.616</v>
+        <v>377</v>
       </c>
       <c r="Q6" t="n">
         <v>397</v>
@@ -11976,13 +11976,13 @@
         <v>419.207</v>
       </c>
       <c r="S6" t="n">
-        <v>438.641</v>
+        <v>515</v>
       </c>
       <c r="T6" t="n">
-        <v>555.463</v>
+        <v>577</v>
       </c>
       <c r="U6" t="n">
-        <v>597.296</v>
+        <v>660</v>
       </c>
       <c r="V6" t="n">
         <v>684.5599999999999</v>
@@ -12047,13 +12047,13 @@
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>12.166</v>
+        <v>162</v>
       </c>
       <c r="Q7" t="n">
         <v>179.81</v>
       </c>
       <c r="R7" t="n">
-        <v>194.81</v>
+        <v>279</v>
       </c>
       <c r="S7" t="n">
         <v>295.325</v>
@@ -12065,10 +12065,10 @@
         <v>330.458</v>
       </c>
       <c r="V7" t="n">
-        <v>352.5</v>
+        <v>501</v>
       </c>
       <c r="W7" t="n">
-        <v>550.115</v>
+        <v>581</v>
       </c>
       <c r="X7" t="n">
         <v>609.111</v>
@@ -12130,7 +12130,7 @@
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>14.866</v>
+        <v>92</v>
       </c>
       <c r="P8" t="n">
         <v>105.606</v>
@@ -12139,13 +12139,13 @@
         <v>117.842</v>
       </c>
       <c r="R8" t="n">
-        <v>130.078</v>
+        <v>333</v>
       </c>
       <c r="S8" t="n">
-        <v>348.657</v>
+        <v>376</v>
       </c>
       <c r="T8" t="n">
-        <v>396.296</v>
+        <v>436</v>
       </c>
       <c r="U8" t="n">
         <v>460.765</v>
@@ -12204,13 +12204,13 @@
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>15</v>
+        <v>228</v>
       </c>
       <c r="N9" t="n">
-        <v>245.071</v>
+        <v>290</v>
       </c>
       <c r="O9" t="n">
-        <v>310</v>
+        <v>388</v>
       </c>
       <c r="P9" t="n">
         <v>403.657</v>
@@ -12260,10 +12260,10 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>18</v>
+        <v>143</v>
       </c>
       <c r="J10" t="n">
-        <v>160.071</v>
+        <v>420</v>
       </c>
       <c r="K10" t="n">
         <v>447.804</v>
@@ -12310,16 +12310,16 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>18.028</v>
+        <v>214</v>
       </c>
       <c r="L11" t="n">
-        <v>233.849</v>
+        <v>236</v>
       </c>
       <c r="M11" t="n">
         <v>254.485</v>
       </c>
       <c r="N11" t="n">
-        <v>276.485</v>
+        <v>294</v>
       </c>
       <c r="O11" t="n">
         <v>362.189</v>
@@ -12375,16 +12375,16 @@
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>20.616</v>
+        <v>34</v>
       </c>
       <c r="O12" t="n">
-        <v>51.071</v>
+        <v>96</v>
       </c>
       <c r="P12" t="n">
         <v>114.062</v>
       </c>
       <c r="Q12" t="n">
-        <v>136.79</v>
+        <v>162</v>
       </c>
       <c r="R12" t="n">
         <v>183.402</v>
@@ -12431,10 +12431,10 @@
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>21.26</v>
+        <v>183</v>
       </c>
       <c r="I13" t="n">
-        <v>202.055</v>
+        <v>272</v>
       </c>
       <c r="J13" t="n">
         <v>288.083</v>
@@ -12472,13 +12472,13 @@
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>22.472</v>
+        <v>31</v>
       </c>
       <c r="J14" t="n">
         <v>54.601</v>
       </c>
       <c r="K14" t="n">
-        <v>94.866</v>
+        <v>190</v>
       </c>
       <c r="L14" t="n">
         <v>250.249</v>
@@ -12516,7 +12516,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>24.759</v>
+        <v>45</v>
       </c>
       <c r="J15" t="n">
         <v>81.571</v>

</xml_diff>